<commit_message>
adding endpoints to fetch sheet names and post new rows
</commit_message>
<xml_diff>
--- a/form-submission-book.xlsx
+++ b/form-submission-book.xlsx
@@ -3,23 +3,32 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17440" windowWidth="28040" xWindow="3260" yWindow="2160"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17440" windowWidth="28040" xWindow="3240" yWindow="2160"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="testSheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="testSheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="181029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="12"/>
       <scheme val="minor"/>
@@ -33,7 +42,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -41,12 +50,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -424,25 +452,240 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" customHeight="1" defaultColWidth="35.83203125" defaultRowHeight="30"/>
+  <cols>
+    <col customWidth="1" max="16384" min="1" style="3" width="35.83203125"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" customHeight="1" ht="30" r="1" s="4">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>site</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>Downtown</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Bryce Eppler</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>status goes here</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>12/06/2022:15:64:12PST</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>Today was a good day for all the guys at work :)</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Downtown</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Bryce Eppler</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>status goes here</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>12/06/2022:15:64:12PST</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>Today was a good day for all the guys at work :)</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Downtown</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Bryce Eppler</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>status goes here</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>12/06/2022:15:64:12PST</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>Today was a good day for all the guys at work :)</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Downtown</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Bryce Eppler</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>status goes here</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>12/06/2022:15:64:12PST</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>Today was a good day for all the guys at work :)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col customWidth="1" max="5" min="5" width="15.33203125"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Hello World</t>
+    <row customFormat="1" r="1" s="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Site</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tasks Completed</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Date</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Hello World</t>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Downtown</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Bryce Eppler</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>status goes here</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>12/06/2022:15:64:12PST</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Today was a good day for all the guys at work :)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adding quickstart script for google sheets api
</commit_message>
<xml_diff>
--- a/form-submission-book.xlsx
+++ b/form-submission-book.xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17440" windowWidth="28040" xWindow="3240" yWindow="2160"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3240" yWindow="2160" windowWidth="28040" windowHeight="17440" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="testSheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="testSheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="DailySiteReport" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="WeeklyStaffReport" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -61,25 +61,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -452,154 +452,109 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A2:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" customHeight="1" defaultColWidth="35.83203125" defaultRowHeight="30"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="35.83203125" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col customWidth="1" max="16384" min="1" style="3" width="35.83203125"/>
+    <col width="35.83203125" customWidth="1" style="3" min="1" max="3"/>
+    <col width="35.83203125" customWidth="1" style="3" min="4" max="16384"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="30" r="1" s="4">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
-        <is>
-          <t>comment</t>
+    <row r="1" ht="30" customFormat="1" customHeight="1" s="4"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Robson St</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Bryce Eppler</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Laying pipe</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>12/13/1999</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Today was a good day for the boys ya know haha</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>Downtown</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DailySite</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Bryce Eppler</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>status goes here</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>12/06/2022:15:64:12PST</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>Today was a good day for all the guys at work :)</t>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>12/54/1024</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>comment penis</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>Downtown</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
+    <row r="4">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Bryce Eppler</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>status goes here</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>12/06/2022:15:64:12PST</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>Today was a good day for all the guys at work :)</t>
-        </is>
-      </c>
     </row>
-    <row customHeight="1" ht="30" r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>Downtown</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Bryce Eppler</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>status goes here</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>12/06/2022:15:64:12PST</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>Today was a good day for all the guys at work :)</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>Downtown</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>Bryce Eppler</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>status goes here</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>12/06/2022:15:64:12PST</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>Today was a good day for all the guys at work :)</t>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -609,87 +564,48 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col customWidth="1" max="5" min="5" width="15.33203125"/>
+    <col width="15.33203125" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Site</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Tasks Completed</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Comments</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
+    <row r="1" customFormat="1" s="1">
+      <c r="F1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Downtown</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>test site</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Bryce Eppler</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>status goes here</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>12/06/2022:15:64:12PST</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Today was a good day for all the guys at work :)</t>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>comment</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>